<commit_message>
Update BE excel instances
</commit_message>
<xml_diff>
--- a/earlywarning-pom/earlywarning-config/src/baf-instances/21_Inst_Variable_BE.xlsx
+++ b/earlywarning-pom/earlywarning-config/src/baf-instances/21_Inst_Variable_BE.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="26520" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="991" activeTab="1"/>
+    <workbookView xWindow="26520" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="991"/>
   </bookViews>
   <sheets>
     <sheet name="Variable" sheetId="1" r:id="rId1"/>
@@ -45,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="171" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="184" uniqueCount="57">
   <si>
     <t>Variable</t>
   </si>
@@ -194,9 +194,6 @@
     <t>BE_SNDG_STRING</t>
   </si>
   <si>
-    <t>BE_TARGET_STRING</t>
-  </si>
-  <si>
     <t>VariableType</t>
   </si>
   <si>
@@ -204,6 +201,21 @@
   </si>
   <si>
     <t>CONTINUOUS</t>
+  </si>
+  <si>
+    <t>BE_IND_3</t>
+  </si>
+  <si>
+    <t>IND_3</t>
+  </si>
+  <si>
+    <t>BE_IND_3_STRING</t>
+  </si>
+  <si>
+    <t>BE_TARGET_REAL</t>
+  </si>
+  <si>
+    <t>3-Descr AFU</t>
   </si>
 </sst>
 </file>
@@ -1336,10 +1348,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K4"/>
+  <dimension ref="A1:K5"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1351,7 +1363,7 @@
     <col min="5" max="6" width="17.5703125"/>
     <col min="7" max="7" width="15.42578125" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="16.7109375" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="15.42578125" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="49" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="16.7109375" bestFit="1" customWidth="1"/>
     <col min="12" max="1023" width="8.7109375"/>
@@ -1401,7 +1413,7 @@
         <v>7</v>
       </c>
       <c r="J2" s="4" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="K2" s="4" t="s">
         <v>8</v>
@@ -1427,7 +1439,7 @@
         <v>42</v>
       </c>
       <c r="G3" s="6">
-        <v>15</v>
+        <v>200</v>
       </c>
       <c r="H3" s="5" t="s">
         <v>13</v>
@@ -1436,7 +1448,7 @@
         <v>13</v>
       </c>
       <c r="J3" s="5" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="K3" s="5" t="s">
         <v>13</v>
@@ -1462,7 +1474,7 @@
         <v>44</v>
       </c>
       <c r="G4" s="6">
-        <v>16</v>
+        <v>201</v>
       </c>
       <c r="H4" s="5" t="s">
         <v>12</v>
@@ -1471,10 +1483,45 @@
         <v>12</v>
       </c>
       <c r="J4" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="K4" s="5" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A5" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="B5" t="s">
         <v>52</v>
       </c>
-      <c r="K4" s="5" t="s">
-        <v>12</v>
+      <c r="C5" t="s">
+        <v>52</v>
+      </c>
+      <c r="D5" t="s">
+        <v>52</v>
+      </c>
+      <c r="E5" t="s">
+        <v>53</v>
+      </c>
+      <c r="F5" t="s">
+        <v>56</v>
+      </c>
+      <c r="G5">
+        <v>3</v>
+      </c>
+      <c r="H5" t="b">
+        <v>0</v>
+      </c>
+      <c r="I5" t="b">
+        <v>0</v>
+      </c>
+      <c r="J5" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="K5" s="5" t="s">
+        <v>13</v>
       </c>
     </row>
   </sheetData>
@@ -1486,10 +1533,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F4"/>
+  <dimension ref="A1:F5"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1554,16 +1601,33 @@
         <v>11</v>
       </c>
       <c r="B4" t="s">
-        <v>49</v>
+        <v>55</v>
       </c>
       <c r="C4" t="s">
-        <v>49</v>
+        <v>55</v>
       </c>
       <c r="E4" s="2" t="s">
         <v>47</v>
       </c>
       <c r="F4" s="2" t="s">
         <v>45</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>11</v>
+      </c>
+      <c r="B5" t="s">
+        <v>54</v>
+      </c>
+      <c r="C5" t="s">
+        <v>54</v>
+      </c>
+      <c r="E5" t="s">
+        <v>52</v>
+      </c>
+      <c r="F5" t="s">
+        <v>23</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Aggiornamento Variable e AnalysisUnit per BE
</commit_message>
<xml_diff>
--- a/earlywarning-pom/earlywarning-config/src/baf-instances/21_Inst_Variable_BE.xlsx
+++ b/earlywarning-pom/earlywarning-config/src/baf-instances/21_Inst_Variable_BE.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Dati\DEV\GitRepoAAAP\client-intesa\earlywarning-pom\earlywarning-config\src\baf-instances\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\giustino.matteo\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="26520" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="991"/>
+    <workbookView xWindow="26520" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="991" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Variable" sheetId="1" r:id="rId1"/>
@@ -45,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="184" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="379" uniqueCount="117">
   <si>
     <t>Variable</t>
   </si>
@@ -215,19 +215,206 @@
     <t>BE_TARGET_REAL</t>
   </si>
   <si>
-    <t>3-Descr AFU</t>
+    <t>IND_7</t>
+  </si>
+  <si>
+    <t>IND_8</t>
+  </si>
+  <si>
+    <t>IND_9</t>
+  </si>
+  <si>
+    <t>IND_14</t>
+  </si>
+  <si>
+    <t>IND_16</t>
+  </si>
+  <si>
+    <t>BE_IND_1</t>
+  </si>
+  <si>
+    <t>BE_IND_2</t>
+  </si>
+  <si>
+    <t>BE_IND_7</t>
+  </si>
+  <si>
+    <t>BE_IND_8</t>
+  </si>
+  <si>
+    <t>BE_IND_9</t>
+  </si>
+  <si>
+    <t>BE_IND_14</t>
+  </si>
+  <si>
+    <t>BE_IND_16</t>
+  </si>
+  <si>
+    <t>BE_IND_34</t>
+  </si>
+  <si>
+    <t>BE_IND_35</t>
+  </si>
+  <si>
+    <t>BE_IND_40</t>
+  </si>
+  <si>
+    <t>BE_IND_44</t>
+  </si>
+  <si>
+    <t>BE_IND_48</t>
+  </si>
+  <si>
+    <t>BE_IND_51</t>
+  </si>
+  <si>
+    <t>BE_IND_55</t>
+  </si>
+  <si>
+    <t>BE_IND_56</t>
+  </si>
+  <si>
+    <t>IND_1</t>
+  </si>
+  <si>
+    <t>IND_2</t>
+  </si>
+  <si>
+    <t>IND_34</t>
+  </si>
+  <si>
+    <t>IND_35</t>
+  </si>
+  <si>
+    <t>IND_40</t>
+  </si>
+  <si>
+    <t>IND_44</t>
+  </si>
+  <si>
+    <t>IND_48</t>
+  </si>
+  <si>
+    <t>IND_51</t>
+  </si>
+  <si>
+    <t>IND_55</t>
+  </si>
+  <si>
+    <t>IND_56</t>
+  </si>
+  <si>
+    <t>1 - Days past due</t>
+  </si>
+  <si>
+    <t>3 - Blocked accounts</t>
+  </si>
+  <si>
+    <t>7 - Overdue amount/exposure amount</t>
+  </si>
+  <si>
+    <t>16 - Default</t>
+  </si>
+  <si>
+    <t>44 - Past due amount</t>
+  </si>
+  <si>
+    <t>56 - Outstanding + overdue/Approved amount for loans</t>
+  </si>
+  <si>
+    <t>2 - Past Due &gt; 90</t>
+  </si>
+  <si>
+    <t>9 - Delta turnover</t>
+  </si>
+  <si>
+    <t>35 - Delta equity</t>
+  </si>
+  <si>
+    <t>48 - Debt Service Coverage Ratio</t>
+  </si>
+  <si>
+    <t>51 - Overdraft</t>
+  </si>
+  <si>
+    <t>55 - Forborne NPE</t>
+  </si>
+  <si>
+    <t>8 - Account turnover oscillation</t>
+  </si>
+  <si>
+    <t xml:space="preserve">14 - Number of business current accounts </t>
+  </si>
+  <si>
+    <t>34 - Negative own equity</t>
+  </si>
+  <si>
+    <t>40 - Loan to value ratio</t>
+  </si>
+  <si>
+    <t>BE_IND_2_STRING</t>
+  </si>
+  <si>
+    <t>BE_IND_16_STRING</t>
+  </si>
+  <si>
+    <t>BE_IND_9_STRING</t>
+  </si>
+  <si>
+    <t>BE_IND_34_STRING</t>
+  </si>
+  <si>
+    <t>BE_IND_51_STRING</t>
+  </si>
+  <si>
+    <t>BE_IND_1_REAL</t>
+  </si>
+  <si>
+    <t>BE_IND_7_REAL</t>
+  </si>
+  <si>
+    <t>BE_IND_8_REAL</t>
+  </si>
+  <si>
+    <t>BE_IND_14_REAL</t>
+  </si>
+  <si>
+    <t>BE_IND_35_REAL</t>
+  </si>
+  <si>
+    <t>BE_IND_40_REAL</t>
+  </si>
+  <si>
+    <t>BE_IND_44_REAL</t>
+  </si>
+  <si>
+    <t>BE_IND_48_REAL</t>
+  </si>
+  <si>
+    <t>BE_IND_55_REAL</t>
+  </si>
+  <si>
+    <t>BE_IND_56_REAL</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
@@ -309,20 +496,21 @@
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="49" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="3" fontId="8" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyFont="1"/>
-    <xf numFmtId="3" fontId="7" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1348,10 +1536,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K5"/>
+  <dimension ref="A1:K20"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+    <sheetView topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B24" sqref="B24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1490,37 +1678,562 @@
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A5" s="5" t="s">
+      <c r="A5" s="7" t="s">
         <v>11</v>
       </c>
       <c r="B5" t="s">
+        <v>61</v>
+      </c>
+      <c r="C5" t="s">
+        <v>61</v>
+      </c>
+      <c r="D5" t="s">
+        <v>61</v>
+      </c>
+      <c r="E5" t="s">
+        <v>76</v>
+      </c>
+      <c r="F5" t="s">
+        <v>86</v>
+      </c>
+      <c r="G5">
+        <v>1</v>
+      </c>
+      <c r="H5" t="b">
+        <v>0</v>
+      </c>
+      <c r="I5" t="b">
+        <v>0</v>
+      </c>
+      <c r="J5" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="K5" s="7" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A6" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="B6" t="s">
+        <v>62</v>
+      </c>
+      <c r="C6" t="s">
+        <v>62</v>
+      </c>
+      <c r="D6" t="s">
+        <v>62</v>
+      </c>
+      <c r="E6" t="s">
+        <v>77</v>
+      </c>
+      <c r="F6" t="s">
+        <v>92</v>
+      </c>
+      <c r="G6">
+        <v>2</v>
+      </c>
+      <c r="H6" t="b">
+        <v>0</v>
+      </c>
+      <c r="I6" t="b">
+        <v>0</v>
+      </c>
+      <c r="J6" s="7" t="s">
+        <v>50</v>
+      </c>
+      <c r="K6" s="7" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A7" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="B7" t="s">
         <v>52</v>
       </c>
-      <c r="C5" t="s">
+      <c r="C7" t="s">
         <v>52</v>
       </c>
-      <c r="D5" t="s">
+      <c r="D7" t="s">
         <v>52</v>
       </c>
-      <c r="E5" t="s">
+      <c r="E7" t="s">
         <v>53</v>
       </c>
-      <c r="F5" t="s">
+      <c r="F7" t="s">
+        <v>87</v>
+      </c>
+      <c r="G7">
+        <v>3</v>
+      </c>
+      <c r="H7" t="b">
+        <v>0</v>
+      </c>
+      <c r="I7" t="b">
+        <v>0</v>
+      </c>
+      <c r="J7" s="7" t="s">
+        <v>50</v>
+      </c>
+      <c r="K7" s="7" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A8" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="B8" t="s">
+        <v>63</v>
+      </c>
+      <c r="C8" t="s">
+        <v>63</v>
+      </c>
+      <c r="D8" t="s">
+        <v>63</v>
+      </c>
+      <c r="E8" t="s">
         <v>56</v>
       </c>
-      <c r="G5">
-        <v>3</v>
-      </c>
-      <c r="H5" t="b">
-        <v>0</v>
-      </c>
-      <c r="I5" t="b">
-        <v>0</v>
-      </c>
-      <c r="J5" s="5" t="s">
+      <c r="F8" t="s">
+        <v>88</v>
+      </c>
+      <c r="G8">
+        <v>7</v>
+      </c>
+      <c r="H8" t="b">
+        <v>0</v>
+      </c>
+      <c r="I8" t="b">
+        <v>0</v>
+      </c>
+      <c r="J8" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="K8" s="7" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A9" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="B9" t="s">
+        <v>64</v>
+      </c>
+      <c r="C9" t="s">
+        <v>64</v>
+      </c>
+      <c r="D9" t="s">
+        <v>64</v>
+      </c>
+      <c r="E9" t="s">
+        <v>57</v>
+      </c>
+      <c r="F9" t="s">
+        <v>98</v>
+      </c>
+      <c r="G9">
+        <v>8</v>
+      </c>
+      <c r="H9" t="b">
+        <v>0</v>
+      </c>
+      <c r="I9" t="b">
+        <v>0</v>
+      </c>
+      <c r="J9" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="K9" s="7" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A10" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="B10" t="s">
+        <v>65</v>
+      </c>
+      <c r="C10" t="s">
+        <v>65</v>
+      </c>
+      <c r="D10" t="s">
+        <v>65</v>
+      </c>
+      <c r="E10" t="s">
+        <v>58</v>
+      </c>
+      <c r="F10" t="s">
+        <v>93</v>
+      </c>
+      <c r="G10">
+        <v>9</v>
+      </c>
+      <c r="H10" t="b">
+        <v>0</v>
+      </c>
+      <c r="I10" t="b">
+        <v>0</v>
+      </c>
+      <c r="J10" s="7" t="s">
         <v>50</v>
       </c>
-      <c r="K5" s="5" t="s">
+      <c r="K10" s="7" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A11" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="B11" t="s">
+        <v>66</v>
+      </c>
+      <c r="C11" t="s">
+        <v>66</v>
+      </c>
+      <c r="D11" t="s">
+        <v>66</v>
+      </c>
+      <c r="E11" t="s">
+        <v>59</v>
+      </c>
+      <c r="F11" t="s">
+        <v>99</v>
+      </c>
+      <c r="G11">
+        <v>14</v>
+      </c>
+      <c r="H11" t="b">
+        <v>0</v>
+      </c>
+      <c r="I11" t="b">
+        <v>0</v>
+      </c>
+      <c r="J11" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="K11" s="7" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A12" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="B12" t="s">
+        <v>67</v>
+      </c>
+      <c r="C12" t="s">
+        <v>67</v>
+      </c>
+      <c r="D12" t="s">
+        <v>67</v>
+      </c>
+      <c r="E12" t="s">
+        <v>60</v>
+      </c>
+      <c r="F12" t="s">
+        <v>89</v>
+      </c>
+      <c r="G12">
+        <v>16</v>
+      </c>
+      <c r="H12" t="b">
+        <v>0</v>
+      </c>
+      <c r="I12" t="b">
+        <v>0</v>
+      </c>
+      <c r="J12" s="7" t="s">
+        <v>50</v>
+      </c>
+      <c r="K12" s="7" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A13" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="B13" t="s">
+        <v>68</v>
+      </c>
+      <c r="C13" t="s">
+        <v>68</v>
+      </c>
+      <c r="D13" t="s">
+        <v>68</v>
+      </c>
+      <c r="E13" t="s">
+        <v>78</v>
+      </c>
+      <c r="F13" t="s">
+        <v>100</v>
+      </c>
+      <c r="G13">
+        <v>34</v>
+      </c>
+      <c r="H13" t="b">
+        <v>0</v>
+      </c>
+      <c r="I13" t="b">
+        <v>0</v>
+      </c>
+      <c r="J13" s="7" t="s">
+        <v>50</v>
+      </c>
+      <c r="K13" s="7" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A14" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="B14" t="s">
+        <v>69</v>
+      </c>
+      <c r="C14" t="s">
+        <v>69</v>
+      </c>
+      <c r="D14" t="s">
+        <v>69</v>
+      </c>
+      <c r="E14" t="s">
+        <v>79</v>
+      </c>
+      <c r="F14" t="s">
+        <v>94</v>
+      </c>
+      <c r="G14">
+        <v>35</v>
+      </c>
+      <c r="H14" t="b">
+        <v>0</v>
+      </c>
+      <c r="I14" t="b">
+        <v>0</v>
+      </c>
+      <c r="J14" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="K14" s="7" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A15" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="B15" t="s">
+        <v>70</v>
+      </c>
+      <c r="C15" t="s">
+        <v>70</v>
+      </c>
+      <c r="D15" t="s">
+        <v>70</v>
+      </c>
+      <c r="E15" t="s">
+        <v>80</v>
+      </c>
+      <c r="F15" t="s">
+        <v>101</v>
+      </c>
+      <c r="G15">
+        <v>40</v>
+      </c>
+      <c r="H15" t="b">
+        <v>0</v>
+      </c>
+      <c r="I15" t="b">
+        <v>0</v>
+      </c>
+      <c r="J15" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="K15" s="7" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A16" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="B16" t="s">
+        <v>71</v>
+      </c>
+      <c r="C16" t="s">
+        <v>71</v>
+      </c>
+      <c r="D16" t="s">
+        <v>71</v>
+      </c>
+      <c r="E16" t="s">
+        <v>81</v>
+      </c>
+      <c r="F16" t="s">
+        <v>90</v>
+      </c>
+      <c r="G16">
+        <v>44</v>
+      </c>
+      <c r="H16" t="b">
+        <v>0</v>
+      </c>
+      <c r="I16" t="b">
+        <v>0</v>
+      </c>
+      <c r="J16" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="K16" s="7" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A17" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="B17" t="s">
+        <v>72</v>
+      </c>
+      <c r="C17" t="s">
+        <v>72</v>
+      </c>
+      <c r="D17" t="s">
+        <v>72</v>
+      </c>
+      <c r="E17" t="s">
+        <v>82</v>
+      </c>
+      <c r="F17" t="s">
+        <v>95</v>
+      </c>
+      <c r="G17">
+        <v>48</v>
+      </c>
+      <c r="H17" t="b">
+        <v>0</v>
+      </c>
+      <c r="I17" t="b">
+        <v>0</v>
+      </c>
+      <c r="J17" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="K17" s="7" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A18" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="B18" t="s">
+        <v>73</v>
+      </c>
+      <c r="C18" t="s">
+        <v>73</v>
+      </c>
+      <c r="D18" t="s">
+        <v>73</v>
+      </c>
+      <c r="E18" t="s">
+        <v>83</v>
+      </c>
+      <c r="F18" t="s">
+        <v>96</v>
+      </c>
+      <c r="G18">
+        <v>51</v>
+      </c>
+      <c r="H18" t="b">
+        <v>0</v>
+      </c>
+      <c r="I18" t="b">
+        <v>0</v>
+      </c>
+      <c r="J18" s="7" t="s">
+        <v>50</v>
+      </c>
+      <c r="K18" s="7" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A19" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="B19" t="s">
+        <v>74</v>
+      </c>
+      <c r="C19" t="s">
+        <v>74</v>
+      </c>
+      <c r="D19" t="s">
+        <v>74</v>
+      </c>
+      <c r="E19" t="s">
+        <v>84</v>
+      </c>
+      <c r="F19" t="s">
+        <v>97</v>
+      </c>
+      <c r="G19">
+        <v>55</v>
+      </c>
+      <c r="H19" t="b">
+        <v>0</v>
+      </c>
+      <c r="I19" t="b">
+        <v>0</v>
+      </c>
+      <c r="J19" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="K19" s="7" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A20" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="B20" t="s">
+        <v>75</v>
+      </c>
+      <c r="C20" t="s">
+        <v>75</v>
+      </c>
+      <c r="D20" t="s">
+        <v>75</v>
+      </c>
+      <c r="E20" t="s">
+        <v>85</v>
+      </c>
+      <c r="F20" t="s">
+        <v>91</v>
+      </c>
+      <c r="G20">
+        <v>56</v>
+      </c>
+      <c r="H20" t="b">
+        <v>0</v>
+      </c>
+      <c r="I20" t="b">
+        <v>0</v>
+      </c>
+      <c r="J20" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="K20" s="7" t="s">
         <v>13</v>
       </c>
     </row>
@@ -1533,10 +2246,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F5"/>
+  <dimension ref="A1:F20"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A11" activeCellId="3" sqref="A21:XFD21 A20:XFD20 A14:XFD14 A11:XFD11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1618,16 +2331,271 @@
         <v>11</v>
       </c>
       <c r="B5" t="s">
+        <v>107</v>
+      </c>
+      <c r="C5" t="s">
+        <v>107</v>
+      </c>
+      <c r="E5" t="s">
+        <v>61</v>
+      </c>
+      <c r="F5" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>11</v>
+      </c>
+      <c r="B6" t="s">
+        <v>102</v>
+      </c>
+      <c r="C6" t="s">
+        <v>102</v>
+      </c>
+      <c r="E6" t="s">
+        <v>62</v>
+      </c>
+      <c r="F6" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>11</v>
+      </c>
+      <c r="B7" t="s">
         <v>54</v>
       </c>
-      <c r="C5" t="s">
+      <c r="C7" t="s">
         <v>54</v>
       </c>
-      <c r="E5" t="s">
+      <c r="E7" t="s">
         <v>52</v>
       </c>
-      <c r="F5" t="s">
+      <c r="F7" t="s">
         <v>23</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>11</v>
+      </c>
+      <c r="B8" t="s">
+        <v>108</v>
+      </c>
+      <c r="C8" t="s">
+        <v>108</v>
+      </c>
+      <c r="E8" t="s">
+        <v>63</v>
+      </c>
+      <c r="F8" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>11</v>
+      </c>
+      <c r="B9" t="s">
+        <v>109</v>
+      </c>
+      <c r="C9" t="s">
+        <v>109</v>
+      </c>
+      <c r="E9" t="s">
+        <v>64</v>
+      </c>
+      <c r="F9" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>11</v>
+      </c>
+      <c r="B10" t="s">
+        <v>104</v>
+      </c>
+      <c r="C10" t="s">
+        <v>104</v>
+      </c>
+      <c r="E10" t="s">
+        <v>65</v>
+      </c>
+      <c r="F10" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>11</v>
+      </c>
+      <c r="B11" t="s">
+        <v>110</v>
+      </c>
+      <c r="C11" t="s">
+        <v>110</v>
+      </c>
+      <c r="E11" t="s">
+        <v>66</v>
+      </c>
+      <c r="F11" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>11</v>
+      </c>
+      <c r="B12" t="s">
+        <v>103</v>
+      </c>
+      <c r="C12" t="s">
+        <v>103</v>
+      </c>
+      <c r="E12" t="s">
+        <v>67</v>
+      </c>
+      <c r="F12" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>11</v>
+      </c>
+      <c r="B13" t="s">
+        <v>105</v>
+      </c>
+      <c r="C13" t="s">
+        <v>105</v>
+      </c>
+      <c r="E13" t="s">
+        <v>68</v>
+      </c>
+      <c r="F13" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>11</v>
+      </c>
+      <c r="B14" t="s">
+        <v>111</v>
+      </c>
+      <c r="C14" t="s">
+        <v>111</v>
+      </c>
+      <c r="E14" t="s">
+        <v>69</v>
+      </c>
+      <c r="F14" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>11</v>
+      </c>
+      <c r="B15" t="s">
+        <v>112</v>
+      </c>
+      <c r="C15" t="s">
+        <v>112</v>
+      </c>
+      <c r="E15" t="s">
+        <v>70</v>
+      </c>
+      <c r="F15" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>11</v>
+      </c>
+      <c r="B16" t="s">
+        <v>113</v>
+      </c>
+      <c r="C16" t="s">
+        <v>113</v>
+      </c>
+      <c r="E16" t="s">
+        <v>71</v>
+      </c>
+      <c r="F16" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>11</v>
+      </c>
+      <c r="B17" t="s">
+        <v>114</v>
+      </c>
+      <c r="C17" t="s">
+        <v>114</v>
+      </c>
+      <c r="E17" t="s">
+        <v>72</v>
+      </c>
+      <c r="F17" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>11</v>
+      </c>
+      <c r="B18" t="s">
+        <v>106</v>
+      </c>
+      <c r="C18" t="s">
+        <v>106</v>
+      </c>
+      <c r="E18" t="s">
+        <v>73</v>
+      </c>
+      <c r="F18" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>11</v>
+      </c>
+      <c r="B19" t="s">
+        <v>115</v>
+      </c>
+      <c r="C19" t="s">
+        <v>115</v>
+      </c>
+      <c r="E19" t="s">
+        <v>74</v>
+      </c>
+      <c r="F19" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>11</v>
+      </c>
+      <c r="B20" t="s">
+        <v>116</v>
+      </c>
+      <c r="C20" t="s">
+        <v>116</v>
+      </c>
+      <c r="E20" t="s">
+        <v>75</v>
+      </c>
+      <c r="F20" t="s">
+        <v>22</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Aggiornamento Variable, Analysis Unit e Workspace
</commit_message>
<xml_diff>
--- a/earlywarning-pom/earlywarning-config/src/baf-instances/21_Inst_Variable_BE.xlsx
+++ b/earlywarning-pom/earlywarning-config/src/baf-instances/21_Inst_Variable_BE.xlsx
@@ -1,15 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\giustino.matteo\Desktop\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9303"/>
+  <workbookPr/>
   <bookViews>
-    <workbookView xWindow="26520" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="991" activeTab="1"/>
+    <workbookView xWindow="26520" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="991"/>
   </bookViews>
   <sheets>
     <sheet name="Variable" sheetId="1" r:id="rId1"/>
@@ -26,7 +21,7 @@
     <author/>
   </authors>
   <commentList>
-    <comment ref="A2" authorId="0" shapeId="0">
+    <comment ref="A2" authorId="0">
       <text>
         <r>
           <rPr>
@@ -1316,7 +1311,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1351,7 +1346,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1528,7 +1523,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1538,8 +1533,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K20"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B24" sqref="B24"/>
+    <sheetView tabSelected="1" topLeftCell="D1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="K15" sqref="K15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1708,8 +1703,8 @@
       <c r="J5" s="7" t="s">
         <v>51</v>
       </c>
-      <c r="K5" s="7" t="s">
-        <v>13</v>
+      <c r="K5" s="5" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
@@ -1813,8 +1808,8 @@
       <c r="J8" s="7" t="s">
         <v>51</v>
       </c>
-      <c r="K8" s="7" t="s">
-        <v>13</v>
+      <c r="K8" s="5" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
@@ -1848,8 +1843,8 @@
       <c r="J9" s="7" t="s">
         <v>51</v>
       </c>
-      <c r="K9" s="7" t="s">
-        <v>13</v>
+      <c r="K9" s="5" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
@@ -1918,8 +1913,8 @@
       <c r="J11" s="7" t="s">
         <v>51</v>
       </c>
-      <c r="K11" s="7" t="s">
-        <v>13</v>
+      <c r="K11" s="5" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.25">
@@ -2023,8 +2018,8 @@
       <c r="J14" s="7" t="s">
         <v>51</v>
       </c>
-      <c r="K14" s="7" t="s">
-        <v>13</v>
+      <c r="K14" s="5" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.25">
@@ -2058,8 +2053,8 @@
       <c r="J15" s="7" t="s">
         <v>51</v>
       </c>
-      <c r="K15" s="7" t="s">
-        <v>13</v>
+      <c r="K15" s="5" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.25">
@@ -2093,8 +2088,8 @@
       <c r="J16" s="7" t="s">
         <v>51</v>
       </c>
-      <c r="K16" s="7" t="s">
-        <v>13</v>
+      <c r="K16" s="5" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.25">
@@ -2128,8 +2123,8 @@
       <c r="J17" s="7" t="s">
         <v>51</v>
       </c>
-      <c r="K17" s="7" t="s">
-        <v>13</v>
+      <c r="K17" s="5" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.25">
@@ -2198,8 +2193,8 @@
       <c r="J19" s="7" t="s">
         <v>51</v>
       </c>
-      <c r="K19" s="7" t="s">
-        <v>13</v>
+      <c r="K19" s="5" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.25">
@@ -2233,8 +2228,8 @@
       <c r="J20" s="7" t="s">
         <v>51</v>
       </c>
-      <c r="K20" s="7" t="s">
-        <v>13</v>
+      <c r="K20" s="5" t="s">
+        <v>12</v>
       </c>
     </row>
   </sheetData>
@@ -2248,8 +2243,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F20"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A11" activeCellId="3" sqref="A21:XFD21 A20:XFD20 A14:XFD14 A11:XFD11"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Aggiornamento Variable e Analysis Unit
</commit_message>
<xml_diff>
--- a/earlywarning-pom/earlywarning-config/src/baf-instances/21_Inst_Variable_BE.xlsx
+++ b/earlywarning-pom/earlywarning-config/src/baf-instances/21_Inst_Variable_BE.xlsx
@@ -5,11 +5,11 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Dati\DEV\GitRepoAAAP\client-intesa\earlywarning-pom\earlywarning-config\src\baf-instances\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\giustino.matteo\Desktop\Progetto Early Warning\Materials_For_3DayTraining\Git\client-intesa\earlywarning-pom\earlywarning-config\src\baf-instances\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="26520" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="991" activeTab="1"/>
+    <workbookView xWindow="26520" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="991"/>
   </bookViews>
   <sheets>
     <sheet name="Variable" sheetId="1" r:id="rId1"/>
@@ -45,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1511" uniqueCount="466">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1524" uniqueCount="470">
   <si>
     <t>Variable</t>
   </si>
@@ -1443,6 +1443,18 @@
   </si>
   <si>
     <t>BE_SEGMENT_STRING</t>
+  </si>
+  <si>
+    <t>BE_IND_15</t>
+  </si>
+  <si>
+    <t>BE_IND_15_STRING</t>
+  </si>
+  <si>
+    <t>IND_15</t>
+  </si>
+  <si>
+    <t>15 - Overdraft limit utilization</t>
   </si>
 </sst>
 </file>
@@ -2600,10 +2612,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M107"/>
+  <dimension ref="A1:M108"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+    <sheetView tabSelected="1" topLeftCell="G1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="K14" sqref="K14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3097,22 +3109,22 @@
         <v>11</v>
       </c>
       <c r="B13" t="s">
-        <v>67</v>
+        <v>466</v>
       </c>
       <c r="C13" t="s">
-        <v>67</v>
+        <v>466</v>
       </c>
       <c r="D13" t="s">
-        <v>67</v>
+        <v>466</v>
       </c>
       <c r="E13" t="s">
-        <v>60</v>
+        <v>468</v>
       </c>
       <c r="F13" t="s">
-        <v>89</v>
+        <v>469</v>
       </c>
       <c r="G13">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="H13" t="b">
         <v>0</v>
@@ -3138,22 +3150,22 @@
         <v>11</v>
       </c>
       <c r="B14" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C14" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="D14" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="E14" t="s">
-        <v>78</v>
+        <v>60</v>
       </c>
       <c r="F14" t="s">
-        <v>100</v>
+        <v>89</v>
       </c>
       <c r="G14">
-        <v>34</v>
+        <v>16</v>
       </c>
       <c r="H14" t="b">
         <v>0</v>
@@ -3179,22 +3191,22 @@
         <v>11</v>
       </c>
       <c r="B15" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C15" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D15" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="E15" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="F15" t="s">
-        <v>94</v>
+        <v>100</v>
       </c>
       <c r="G15">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="H15" t="b">
         <v>0</v>
@@ -3203,10 +3215,10 @@
         <v>0</v>
       </c>
       <c r="J15" s="7" t="s">
-        <v>51</v>
-      </c>
-      <c r="K15" s="5" t="s">
-        <v>12</v>
+        <v>50</v>
+      </c>
+      <c r="K15" s="7" t="s">
+        <v>13</v>
       </c>
       <c r="L15" t="b">
         <v>0</v>
@@ -3220,22 +3232,22 @@
         <v>11</v>
       </c>
       <c r="B16" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C16" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="D16" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="E16" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="F16" t="s">
-        <v>101</v>
+        <v>94</v>
       </c>
       <c r="G16">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="H16" t="b">
         <v>0</v>
@@ -3261,22 +3273,22 @@
         <v>11</v>
       </c>
       <c r="B17" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C17" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D17" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="E17" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="F17" t="s">
-        <v>90</v>
+        <v>101</v>
       </c>
       <c r="G17">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="H17" t="b">
         <v>0</v>
@@ -3302,22 +3314,22 @@
         <v>11</v>
       </c>
       <c r="B18" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C18" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D18" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="E18" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="F18" t="s">
-        <v>95</v>
+        <v>90</v>
       </c>
       <c r="G18">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="H18" t="b">
         <v>0</v>
@@ -3343,34 +3355,34 @@
         <v>11</v>
       </c>
       <c r="B19" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C19" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="D19" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="E19" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="F19" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="G19">
+        <v>48</v>
+      </c>
+      <c r="H19" t="b">
+        <v>0</v>
+      </c>
+      <c r="I19" t="b">
+        <v>0</v>
+      </c>
+      <c r="J19" s="7" t="s">
         <v>51</v>
       </c>
-      <c r="H19" t="b">
-        <v>0</v>
-      </c>
-      <c r="I19" t="b">
-        <v>0</v>
-      </c>
-      <c r="J19" s="7" t="s">
-        <v>50</v>
-      </c>
-      <c r="K19" s="7" t="s">
-        <v>13</v>
+      <c r="K19" s="5" t="s">
+        <v>12</v>
       </c>
       <c r="L19" t="b">
         <v>0</v>
@@ -3384,22 +3396,22 @@
         <v>11</v>
       </c>
       <c r="B20" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C20" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D20" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="E20" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="F20" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="G20">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="H20" t="b">
         <v>0</v>
@@ -3407,7 +3419,7 @@
       <c r="I20" t="b">
         <v>0</v>
       </c>
-      <c r="J20" s="9" t="s">
+      <c r="J20" s="7" t="s">
         <v>50</v>
       </c>
       <c r="K20" s="7" t="s">
@@ -3425,22 +3437,22 @@
         <v>11</v>
       </c>
       <c r="B21" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C21" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="D21" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="E21" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="F21" t="s">
-        <v>91</v>
+        <v>97</v>
       </c>
       <c r="G21">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="H21" t="b">
         <v>0</v>
@@ -3448,11 +3460,11 @@
       <c r="I21" t="b">
         <v>0</v>
       </c>
-      <c r="J21" s="7" t="s">
-        <v>51</v>
-      </c>
-      <c r="K21" s="5" t="s">
-        <v>12</v>
+      <c r="J21" s="9" t="s">
+        <v>50</v>
+      </c>
+      <c r="K21" s="7" t="s">
+        <v>13</v>
       </c>
       <c r="L21" t="b">
         <v>0</v>
@@ -3466,22 +3478,22 @@
         <v>11</v>
       </c>
       <c r="B22" t="s">
-        <v>115</v>
+        <v>75</v>
       </c>
       <c r="C22" t="s">
-        <v>115</v>
+        <v>75</v>
       </c>
       <c r="D22" t="s">
-        <v>115</v>
+        <v>75</v>
       </c>
       <c r="E22" t="s">
-        <v>200</v>
+        <v>85</v>
       </c>
       <c r="F22" t="s">
-        <v>285</v>
+        <v>91</v>
       </c>
       <c r="G22">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="H22" t="b">
         <v>0</v>
@@ -3507,22 +3519,22 @@
         <v>11</v>
       </c>
       <c r="B23" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="C23" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="D23" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="E23" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="F23" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="G23">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="H23" t="b">
         <v>0</v>
@@ -3548,22 +3560,22 @@
         <v>11</v>
       </c>
       <c r="B24" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="C24" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="D24" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="E24" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="F24" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="G24">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="H24" t="b">
         <v>0</v>
@@ -3589,22 +3601,22 @@
         <v>11</v>
       </c>
       <c r="B25" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="C25" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="D25" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="E25" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="F25" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="G25">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="H25" t="b">
         <v>0</v>
@@ -3630,22 +3642,22 @@
         <v>11</v>
       </c>
       <c r="B26" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="C26" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="D26" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="E26" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="F26" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="G26">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="H26" t="b">
         <v>0</v>
@@ -3671,22 +3683,22 @@
         <v>11</v>
       </c>
       <c r="B27" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="C27" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="D27" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="E27" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="F27" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="G27">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="H27" t="b">
         <v>0</v>
@@ -3712,22 +3724,22 @@
         <v>11</v>
       </c>
       <c r="B28" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="C28" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="D28" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="E28" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="F28" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="G28">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="H28" t="b">
         <v>0</v>
@@ -3753,22 +3765,22 @@
         <v>11</v>
       </c>
       <c r="B29" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="C29" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="D29" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="E29" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="F29" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="G29">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="H29" t="b">
         <v>0</v>
@@ -3794,22 +3806,22 @@
         <v>11</v>
       </c>
       <c r="B30" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="C30" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="D30" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="E30" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="F30" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="G30">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="H30" t="b">
         <v>0</v>
@@ -3835,22 +3847,22 @@
         <v>11</v>
       </c>
       <c r="B31" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="C31" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="D31" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="E31" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="F31" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="G31">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="H31" t="b">
         <v>0</v>
@@ -3876,22 +3888,22 @@
         <v>11</v>
       </c>
       <c r="B32" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="C32" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="D32" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="E32" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="F32" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="G32">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="H32" t="b">
         <v>0</v>
@@ -3917,22 +3929,22 @@
         <v>11</v>
       </c>
       <c r="B33" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="C33" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="D33" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="E33" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="F33" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="G33">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="H33" t="b">
         <v>0</v>
@@ -3958,22 +3970,22 @@
         <v>11</v>
       </c>
       <c r="B34" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="C34" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="D34" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="E34" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="F34" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="G34">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="H34" t="b">
         <v>0</v>
@@ -3999,22 +4011,22 @@
         <v>11</v>
       </c>
       <c r="B35" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C35" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="D35" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="E35" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="F35" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="G35">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="H35" t="b">
         <v>0</v>
@@ -4040,22 +4052,22 @@
         <v>11</v>
       </c>
       <c r="B36" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="C36" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="D36" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="E36" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="F36" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="G36">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="H36" t="b">
         <v>0</v>
@@ -4081,22 +4093,22 @@
         <v>11</v>
       </c>
       <c r="B37" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="C37" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="D37" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="E37" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="F37" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="G37">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="H37" t="b">
         <v>0</v>
@@ -4122,22 +4134,22 @@
         <v>11</v>
       </c>
       <c r="B38" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="C38" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="D38" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="E38" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="F38" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="G38">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="H38" t="b">
         <v>0</v>
@@ -4163,22 +4175,22 @@
         <v>11</v>
       </c>
       <c r="B39" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="C39" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="D39" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="E39" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="F39" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="G39">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="H39" t="b">
         <v>0</v>
@@ -4204,22 +4216,22 @@
         <v>11</v>
       </c>
       <c r="B40" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="C40" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="D40" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="E40" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="F40" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="G40">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="H40" t="b">
         <v>0</v>
@@ -4245,22 +4257,22 @@
         <v>11</v>
       </c>
       <c r="B41" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="C41" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="D41" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="E41" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="F41" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="G41">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="H41" t="b">
         <v>0</v>
@@ -4286,22 +4298,22 @@
         <v>11</v>
       </c>
       <c r="B42" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="C42" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="D42" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="E42" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="F42" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="G42">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="H42" t="b">
         <v>0</v>
@@ -4327,22 +4339,22 @@
         <v>11</v>
       </c>
       <c r="B43" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="C43" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="D43" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="E43" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="F43" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="G43">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="H43" t="b">
         <v>0</v>
@@ -4368,22 +4380,22 @@
         <v>11</v>
       </c>
       <c r="B44" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="C44" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="D44" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="E44" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="F44" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="G44">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="H44" t="b">
         <v>0</v>
@@ -4409,22 +4421,22 @@
         <v>11</v>
       </c>
       <c r="B45" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="C45" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="D45" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="E45" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="F45" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="G45">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="H45" t="b">
         <v>0</v>
@@ -4450,22 +4462,22 @@
         <v>11</v>
       </c>
       <c r="B46" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="C46" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="D46" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="E46" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="F46" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="G46">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="H46" t="b">
         <v>0</v>
@@ -4491,22 +4503,22 @@
         <v>11</v>
       </c>
       <c r="B47" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="C47" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="D47" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="E47" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="F47" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="G47">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="H47" t="b">
         <v>0</v>
@@ -4532,22 +4544,22 @@
         <v>11</v>
       </c>
       <c r="B48" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="C48" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="D48" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="E48" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="F48" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="G48">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="H48" t="b">
         <v>0</v>
@@ -4573,22 +4585,22 @@
         <v>11</v>
       </c>
       <c r="B49" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="C49" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="D49" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="E49" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="F49" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="G49">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="H49" t="b">
         <v>0</v>
@@ -4614,22 +4626,22 @@
         <v>11</v>
       </c>
       <c r="B50" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="C50" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="D50" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="E50" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="F50" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="G50">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="H50" t="b">
         <v>0</v>
@@ -4655,22 +4667,22 @@
         <v>11</v>
       </c>
       <c r="B51" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="C51" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="D51" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="E51" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="F51" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="G51">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="H51" t="b">
         <v>0</v>
@@ -4696,22 +4708,22 @@
         <v>11</v>
       </c>
       <c r="B52" t="s">
-        <v>456</v>
+        <v>144</v>
       </c>
       <c r="C52" t="s">
-        <v>456</v>
+        <v>144</v>
       </c>
       <c r="D52" t="s">
-        <v>456</v>
+        <v>144</v>
       </c>
       <c r="E52" t="s">
-        <v>457</v>
+        <v>229</v>
       </c>
       <c r="F52" t="s">
-        <v>458</v>
+        <v>314</v>
       </c>
       <c r="G52">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="H52" t="b">
         <v>0</v>
@@ -4737,22 +4749,22 @@
         <v>11</v>
       </c>
       <c r="B53" t="s">
-        <v>145</v>
+        <v>456</v>
       </c>
       <c r="C53" t="s">
-        <v>145</v>
+        <v>456</v>
       </c>
       <c r="D53" t="s">
-        <v>145</v>
+        <v>456</v>
       </c>
       <c r="E53" t="s">
-        <v>230</v>
+        <v>457</v>
       </c>
       <c r="F53" t="s">
-        <v>315</v>
+        <v>458</v>
       </c>
       <c r="G53">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="H53" t="b">
         <v>0</v>
@@ -4778,22 +4790,22 @@
         <v>11</v>
       </c>
       <c r="B54" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="C54" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="D54" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="E54" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="F54" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="G54">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="H54" t="b">
         <v>0</v>
@@ -4819,22 +4831,22 @@
         <v>11</v>
       </c>
       <c r="B55" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="C55" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="D55" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="E55" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="F55" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="G55">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="H55" t="b">
         <v>0</v>
@@ -4860,22 +4872,22 @@
         <v>11</v>
       </c>
       <c r="B56" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="C56" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="D56" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="E56" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="F56" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="G56">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="H56" t="b">
         <v>0</v>
@@ -4901,22 +4913,22 @@
         <v>11</v>
       </c>
       <c r="B57" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="C57" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="D57" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="E57" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="F57" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="G57">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="H57" t="b">
         <v>0</v>
@@ -4942,22 +4954,22 @@
         <v>11</v>
       </c>
       <c r="B58" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="C58" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="D58" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="E58" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="F58" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="G58">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="H58" t="b">
         <v>0</v>
@@ -4983,22 +4995,22 @@
         <v>11</v>
       </c>
       <c r="B59" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="C59" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="D59" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="E59" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="F59" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="G59">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="H59" t="b">
         <v>0</v>
@@ -5024,22 +5036,22 @@
         <v>11</v>
       </c>
       <c r="B60" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="C60" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="D60" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="E60" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="F60" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="G60">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="H60" t="b">
         <v>0</v>
@@ -5065,22 +5077,22 @@
         <v>11</v>
       </c>
       <c r="B61" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="C61" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="D61" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="E61" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="F61" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="G61">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="H61" t="b">
         <v>0</v>
@@ -5106,22 +5118,22 @@
         <v>11</v>
       </c>
       <c r="B62" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="C62" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="D62" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="E62" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="F62" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="G62">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="H62" t="b">
         <v>0</v>
@@ -5147,22 +5159,22 @@
         <v>11</v>
       </c>
       <c r="B63" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="C63" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="D63" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="E63" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="F63" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="G63">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="H63" t="b">
         <v>0</v>
@@ -5188,22 +5200,22 @@
         <v>11</v>
       </c>
       <c r="B64" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="C64" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="D64" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="E64" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="F64" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="G64">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="H64" t="b">
         <v>0</v>
@@ -5229,22 +5241,22 @@
         <v>11</v>
       </c>
       <c r="B65" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="C65" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="D65" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="E65" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="F65" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="G65">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="H65" t="b">
         <v>0</v>
@@ -5270,22 +5282,22 @@
         <v>11</v>
       </c>
       <c r="B66" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="C66" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="D66" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="E66" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="F66" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="G66">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="H66" t="b">
         <v>0</v>
@@ -5311,22 +5323,22 @@
         <v>11</v>
       </c>
       <c r="B67" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="C67" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="D67" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="E67" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="F67" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="G67">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="H67" t="b">
         <v>0</v>
@@ -5352,22 +5364,22 @@
         <v>11</v>
       </c>
       <c r="B68" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="C68" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="D68" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="E68" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="F68" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="G68">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="H68" t="b">
         <v>0</v>
@@ -5393,22 +5405,22 @@
         <v>11</v>
       </c>
       <c r="B69" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="C69" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="D69" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="E69" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="F69" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="G69">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="H69" t="b">
         <v>0</v>
@@ -5434,22 +5446,22 @@
         <v>11</v>
       </c>
       <c r="B70" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="C70" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="D70" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="E70" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="F70" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="G70">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="H70" t="b">
         <v>0</v>
@@ -5475,22 +5487,22 @@
         <v>11</v>
       </c>
       <c r="B71" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="C71" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="D71" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="E71" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="F71" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="G71">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="H71" t="b">
         <v>0</v>
@@ -5516,22 +5528,22 @@
         <v>11</v>
       </c>
       <c r="B72" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="C72" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="D72" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="E72" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="F72" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="G72">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="H72" t="b">
         <v>0</v>
@@ -5557,22 +5569,22 @@
         <v>11</v>
       </c>
       <c r="B73" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="C73" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="D73" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="E73" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="F73" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="G73">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="H73" t="b">
         <v>0</v>
@@ -5598,22 +5610,22 @@
         <v>11</v>
       </c>
       <c r="B74" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="C74" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="D74" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="E74" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="F74" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="G74">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="H74" t="b">
         <v>0</v>
@@ -5639,22 +5651,22 @@
         <v>11</v>
       </c>
       <c r="B75" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="C75" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="D75" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="E75" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="F75" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="G75">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="H75" t="b">
         <v>0</v>
@@ -5680,22 +5692,22 @@
         <v>11</v>
       </c>
       <c r="B76" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="C76" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="D76" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="E76" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="F76" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="G76">
-        <v>124</v>
+        <v>120</v>
       </c>
       <c r="H76" t="b">
         <v>0</v>
@@ -5721,22 +5733,22 @@
         <v>11</v>
       </c>
       <c r="B77" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="C77" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="D77" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="E77" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="F77" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="G77">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="H77" t="b">
         <v>0</v>
@@ -5762,22 +5774,22 @@
         <v>11</v>
       </c>
       <c r="B78" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="C78" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="D78" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="E78" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="F78" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="G78">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="H78" t="b">
         <v>0</v>
@@ -5803,22 +5815,22 @@
         <v>11</v>
       </c>
       <c r="B79" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="C79" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="D79" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="E79" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="F79" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="G79">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="H79" t="b">
         <v>0</v>
@@ -5844,22 +5856,22 @@
         <v>11</v>
       </c>
       <c r="B80" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="C80" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="D80" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="E80" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="F80" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="G80">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="H80" t="b">
         <v>0</v>
@@ -5885,22 +5897,22 @@
         <v>11</v>
       </c>
       <c r="B81" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="C81" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="D81" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="E81" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="F81" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="G81">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="H81" t="b">
         <v>0</v>
@@ -5926,22 +5938,22 @@
         <v>11</v>
       </c>
       <c r="B82" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="C82" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="D82" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="E82" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="F82" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="G82">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="H82" t="b">
         <v>0</v>
@@ -5967,22 +5979,22 @@
         <v>11</v>
       </c>
       <c r="B83" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="C83" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="D83" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="E83" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="F83" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="G83">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="H83" t="b">
         <v>0</v>
@@ -6008,22 +6020,22 @@
         <v>11</v>
       </c>
       <c r="B84" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="C84" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="D84" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="E84" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="F84" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="G84">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="H84" t="b">
         <v>0</v>
@@ -6049,22 +6061,22 @@
         <v>11</v>
       </c>
       <c r="B85" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="C85" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="D85" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="E85" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="F85" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="G85">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="H85" t="b">
         <v>0</v>
@@ -6090,22 +6102,22 @@
         <v>11</v>
       </c>
       <c r="B86" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="C86" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="D86" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="E86" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="F86" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="G86">
-        <v>172</v>
+        <v>133</v>
       </c>
       <c r="H86" t="b">
         <v>0</v>
@@ -6114,10 +6126,10 @@
         <v>0</v>
       </c>
       <c r="J86" s="7" t="s">
-        <v>50</v>
-      </c>
-      <c r="K86" s="7" t="s">
-        <v>13</v>
+        <v>51</v>
+      </c>
+      <c r="K86" s="5" t="s">
+        <v>12</v>
       </c>
       <c r="L86" t="b">
         <v>0</v>
@@ -6131,22 +6143,22 @@
         <v>11</v>
       </c>
       <c r="B87" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="C87" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="D87" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="E87" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="F87" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="G87">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="H87" t="b">
         <v>0</v>
@@ -6172,22 +6184,22 @@
         <v>11</v>
       </c>
       <c r="B88" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="C88" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="D88" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="E88" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="F88" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="G88">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="H88" t="b">
         <v>0</v>
@@ -6213,22 +6225,22 @@
         <v>11</v>
       </c>
       <c r="B89" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="C89" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="D89" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="E89" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="F89" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="G89">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="H89" t="b">
         <v>0</v>
@@ -6254,22 +6266,22 @@
         <v>11</v>
       </c>
       <c r="B90" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="C90" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="D90" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="E90" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="F90" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="G90">
-        <v>180</v>
+        <v>175</v>
       </c>
       <c r="H90" t="b">
         <v>0</v>
@@ -6278,10 +6290,10 @@
         <v>0</v>
       </c>
       <c r="J90" s="7" t="s">
-        <v>51</v>
-      </c>
-      <c r="K90" s="5" t="s">
-        <v>12</v>
+        <v>50</v>
+      </c>
+      <c r="K90" s="7" t="s">
+        <v>13</v>
       </c>
       <c r="L90" t="b">
         <v>0</v>
@@ -6295,22 +6307,22 @@
         <v>11</v>
       </c>
       <c r="B91" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="C91" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="D91" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="E91" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="F91" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="G91">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="H91" t="b">
         <v>0</v>
@@ -6336,22 +6348,22 @@
         <v>11</v>
       </c>
       <c r="B92" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="C92" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="D92" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="E92" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="F92" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="G92">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="H92" t="b">
         <v>0</v>
@@ -6377,22 +6389,22 @@
         <v>11</v>
       </c>
       <c r="B93" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="C93" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="D93" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="E93" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="F93" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="G93">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="H93" t="b">
         <v>0</v>
@@ -6418,22 +6430,22 @@
         <v>11</v>
       </c>
       <c r="B94" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="C94" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="D94" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="E94" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="F94" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="G94">
-        <v>186</v>
+        <v>183</v>
       </c>
       <c r="H94" t="b">
         <v>0</v>
@@ -6459,22 +6471,22 @@
         <v>11</v>
       </c>
       <c r="B95" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="C95" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="D95" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="E95" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="F95" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="G95">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="H95" t="b">
         <v>0</v>
@@ -6500,22 +6512,22 @@
         <v>11</v>
       </c>
       <c r="B96" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="C96" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="D96" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="E96" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="F96" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="G96">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="H96" t="b">
         <v>0</v>
@@ -6541,22 +6553,22 @@
         <v>11</v>
       </c>
       <c r="B97" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="C97" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="D97" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="E97" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="F97" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="G97">
-        <v>193</v>
+        <v>188</v>
       </c>
       <c r="H97" t="b">
         <v>0</v>
@@ -6582,22 +6594,22 @@
         <v>11</v>
       </c>
       <c r="B98" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="C98" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="D98" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="E98" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="F98" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="G98">
-        <v>197</v>
+        <v>193</v>
       </c>
       <c r="H98" t="b">
         <v>0</v>
@@ -6623,22 +6635,22 @@
         <v>11</v>
       </c>
       <c r="B99" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="C99" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="D99" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="E99" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="F99" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="G99">
-        <v>201</v>
+        <v>197</v>
       </c>
       <c r="H99" t="b">
         <v>0</v>
@@ -6664,22 +6676,22 @@
         <v>11</v>
       </c>
       <c r="B100" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="C100" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="D100" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="E100" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="F100" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="G100">
-        <v>205</v>
+        <v>201</v>
       </c>
       <c r="H100" t="b">
         <v>0</v>
@@ -6705,22 +6717,22 @@
         <v>11</v>
       </c>
       <c r="B101" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="C101" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="D101" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="E101" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="F101" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="G101">
-        <v>211</v>
+        <v>205</v>
       </c>
       <c r="H101" t="b">
         <v>0</v>
@@ -6746,22 +6758,22 @@
         <v>11</v>
       </c>
       <c r="B102" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="C102" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="D102" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="E102" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="F102" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="G102">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="H102" t="b">
         <v>0</v>
@@ -6787,22 +6799,22 @@
         <v>11</v>
       </c>
       <c r="B103" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="C103" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="D103" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="E103" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="F103" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="G103">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="H103" t="b">
         <v>0</v>
@@ -6828,22 +6840,22 @@
         <v>11</v>
       </c>
       <c r="B104" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="C104" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="D104" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="E104" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="F104" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="G104">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="H104" t="b">
         <v>0</v>
@@ -6869,22 +6881,22 @@
         <v>11</v>
       </c>
       <c r="B105" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="C105" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="D105" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="E105" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="F105" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="G105">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="H105" t="b">
         <v>0</v>
@@ -6910,22 +6922,22 @@
         <v>11</v>
       </c>
       <c r="B106" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="C106" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="D106" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="E106" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="F106" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
       <c r="G106">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="H106" t="b">
         <v>0</v>
@@ -6951,22 +6963,22 @@
         <v>11</v>
       </c>
       <c r="B107" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="C107" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="D107" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="E107" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="F107" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="G107">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="H107" t="b">
         <v>0</v>
@@ -6984,6 +6996,47 @@
         <v>0</v>
       </c>
       <c r="M107" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="108" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A108" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="B108" t="s">
+        <v>199</v>
+      </c>
+      <c r="C108" t="s">
+        <v>199</v>
+      </c>
+      <c r="D108" t="s">
+        <v>199</v>
+      </c>
+      <c r="E108" t="s">
+        <v>284</v>
+      </c>
+      <c r="F108" t="s">
+        <v>369</v>
+      </c>
+      <c r="G108">
+        <v>218</v>
+      </c>
+      <c r="H108" t="b">
+        <v>0</v>
+      </c>
+      <c r="I108" t="b">
+        <v>0</v>
+      </c>
+      <c r="J108" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="K108" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="L108" t="b">
+        <v>0</v>
+      </c>
+      <c r="M108" t="b">
         <v>0</v>
       </c>
     </row>
@@ -6996,10 +7049,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F107"/>
+  <dimension ref="A1:F108"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F1" sqref="F1"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7217,13 +7270,13 @@
         <v>11</v>
       </c>
       <c r="B13" t="s">
-        <v>103</v>
+        <v>467</v>
       </c>
       <c r="C13" t="s">
-        <v>103</v>
+        <v>467</v>
       </c>
       <c r="E13" t="s">
-        <v>67</v>
+        <v>466</v>
       </c>
       <c r="F13" t="s">
         <v>23</v>
@@ -7234,13 +7287,13 @@
         <v>11</v>
       </c>
       <c r="B14" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="C14" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="E14" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="F14" t="s">
         <v>23</v>
@@ -7251,16 +7304,16 @@
         <v>11</v>
       </c>
       <c r="B15" t="s">
-        <v>110</v>
+        <v>104</v>
       </c>
       <c r="C15" t="s">
-        <v>110</v>
+        <v>104</v>
       </c>
       <c r="E15" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="F15" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
@@ -7268,13 +7321,13 @@
         <v>11</v>
       </c>
       <c r="B16" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="C16" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="E16" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="F16" t="s">
         <v>22</v>
@@ -7285,13 +7338,13 @@
         <v>11</v>
       </c>
       <c r="B17" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C17" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="E17" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="F17" t="s">
         <v>22</v>
@@ -7302,13 +7355,13 @@
         <v>11</v>
       </c>
       <c r="B18" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="C18" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="E18" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="F18" t="s">
         <v>22</v>
@@ -7319,16 +7372,16 @@
         <v>11</v>
       </c>
       <c r="B19" t="s">
-        <v>105</v>
+        <v>113</v>
       </c>
       <c r="C19" t="s">
-        <v>105</v>
+        <v>113</v>
       </c>
       <c r="E19" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="F19" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
@@ -7336,15 +7389,15 @@
         <v>11</v>
       </c>
       <c r="B20" t="s">
-        <v>459</v>
+        <v>105</v>
       </c>
       <c r="C20" t="s">
-        <v>459</v>
+        <v>105</v>
       </c>
       <c r="E20" t="s">
-        <v>74</v>
-      </c>
-      <c r="F20" s="8" t="s">
+        <v>73</v>
+      </c>
+      <c r="F20" t="s">
         <v>23</v>
       </c>
     </row>
@@ -7353,16 +7406,16 @@
         <v>11</v>
       </c>
       <c r="B21" t="s">
-        <v>114</v>
+        <v>459</v>
       </c>
       <c r="C21" t="s">
-        <v>114</v>
+        <v>459</v>
       </c>
       <c r="E21" t="s">
-        <v>75</v>
-      </c>
-      <c r="F21" t="s">
-        <v>22</v>
+        <v>74</v>
+      </c>
+      <c r="F21" s="8" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
@@ -7370,13 +7423,13 @@
         <v>11</v>
       </c>
       <c r="B22" t="s">
-        <v>370</v>
+        <v>114</v>
       </c>
       <c r="C22" t="s">
-        <v>370</v>
+        <v>114</v>
       </c>
       <c r="E22" t="s">
-        <v>115</v>
+        <v>75</v>
       </c>
       <c r="F22" t="s">
         <v>22</v>
@@ -7387,13 +7440,13 @@
         <v>11</v>
       </c>
       <c r="B23" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="C23" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="E23" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="F23" t="s">
         <v>22</v>
@@ -7404,13 +7457,13 @@
         <v>11</v>
       </c>
       <c r="B24" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="C24" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="E24" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="F24" t="s">
         <v>22</v>
@@ -7421,13 +7474,13 @@
         <v>11</v>
       </c>
       <c r="B25" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="C25" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="E25" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="F25" t="s">
         <v>22</v>
@@ -7438,13 +7491,13 @@
         <v>11</v>
       </c>
       <c r="B26" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="C26" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="E26" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="F26" t="s">
         <v>22</v>
@@ -7455,13 +7508,13 @@
         <v>11</v>
       </c>
       <c r="B27" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="C27" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="E27" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="F27" t="s">
         <v>22</v>
@@ -7472,13 +7525,13 @@
         <v>11</v>
       </c>
       <c r="B28" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="C28" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="E28" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="F28" t="s">
         <v>22</v>
@@ -7489,13 +7542,13 @@
         <v>11</v>
       </c>
       <c r="B29" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="C29" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="E29" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="F29" t="s">
         <v>22</v>
@@ -7506,13 +7559,13 @@
         <v>11</v>
       </c>
       <c r="B30" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="C30" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="E30" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="F30" t="s">
         <v>22</v>
@@ -7523,13 +7576,13 @@
         <v>11</v>
       </c>
       <c r="B31" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="C31" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="E31" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="F31" t="s">
         <v>22</v>
@@ -7540,13 +7593,13 @@
         <v>11</v>
       </c>
       <c r="B32" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
       <c r="C32" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
       <c r="E32" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="F32" t="s">
         <v>22</v>
@@ -7557,13 +7610,13 @@
         <v>11</v>
       </c>
       <c r="B33" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="C33" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="E33" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="F33" t="s">
         <v>22</v>
@@ -7574,13 +7627,13 @@
         <v>11</v>
       </c>
       <c r="B34" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="C34" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="E34" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="F34" t="s">
         <v>22</v>
@@ -7591,13 +7644,13 @@
         <v>11</v>
       </c>
       <c r="B35" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
       <c r="C35" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
       <c r="E35" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="F35" t="s">
         <v>22</v>
@@ -7608,13 +7661,13 @@
         <v>11</v>
       </c>
       <c r="B36" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="C36" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="E36" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="F36" t="s">
         <v>22</v>
@@ -7625,13 +7678,13 @@
         <v>11</v>
       </c>
       <c r="B37" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="C37" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="E37" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="F37" t="s">
         <v>22</v>
@@ -7642,13 +7695,13 @@
         <v>11</v>
       </c>
       <c r="B38" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="C38" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="E38" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="F38" t="s">
         <v>22</v>
@@ -7659,13 +7712,13 @@
         <v>11</v>
       </c>
       <c r="B39" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="C39" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="E39" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="F39" t="s">
         <v>22</v>
@@ -7676,13 +7729,13 @@
         <v>11</v>
       </c>
       <c r="B40" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="C40" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="E40" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="F40" t="s">
         <v>22</v>
@@ -7693,13 +7746,13 @@
         <v>11</v>
       </c>
       <c r="B41" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="C41" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="E41" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="F41" t="s">
         <v>22</v>
@@ -7710,13 +7763,13 @@
         <v>11</v>
       </c>
       <c r="B42" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="C42" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="E42" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="F42" t="s">
         <v>22</v>
@@ -7727,13 +7780,13 @@
         <v>11</v>
       </c>
       <c r="B43" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="C43" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="E43" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="F43" t="s">
         <v>22</v>
@@ -7744,13 +7797,13 @@
         <v>11</v>
       </c>
       <c r="B44" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="C44" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="E44" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="F44" t="s">
         <v>22</v>
@@ -7761,13 +7814,13 @@
         <v>11</v>
       </c>
       <c r="B45" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="C45" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="E45" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="F45" t="s">
         <v>22</v>
@@ -7778,13 +7831,13 @@
         <v>11</v>
       </c>
       <c r="B46" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="C46" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="E46" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="F46" t="s">
         <v>22</v>
@@ -7795,13 +7848,13 @@
         <v>11</v>
       </c>
       <c r="B47" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="C47" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="E47" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="F47" t="s">
         <v>22</v>
@@ -7812,13 +7865,13 @@
         <v>11</v>
       </c>
       <c r="B48" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="C48" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="E48" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="F48" t="s">
         <v>22</v>
@@ -7829,13 +7882,13 @@
         <v>11</v>
       </c>
       <c r="B49" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
       <c r="C49" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
       <c r="E49" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="F49" t="s">
         <v>22</v>
@@ -7846,13 +7899,13 @@
         <v>11</v>
       </c>
       <c r="B50" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
       <c r="C50" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
       <c r="E50" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="F50" t="s">
         <v>22</v>
@@ -7863,13 +7916,13 @@
         <v>11</v>
       </c>
       <c r="B51" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
       <c r="C51" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
       <c r="E51" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="F51" t="s">
         <v>22</v>
@@ -7880,13 +7933,13 @@
         <v>11</v>
       </c>
       <c r="B52" t="s">
-        <v>455</v>
+        <v>399</v>
       </c>
       <c r="C52" t="s">
-        <v>455</v>
+        <v>399</v>
       </c>
       <c r="E52" t="s">
-        <v>456</v>
+        <v>144</v>
       </c>
       <c r="F52" t="s">
         <v>22</v>
@@ -7897,13 +7950,13 @@
         <v>11</v>
       </c>
       <c r="B53" t="s">
-        <v>400</v>
+        <v>455</v>
       </c>
       <c r="C53" t="s">
-        <v>400</v>
+        <v>455</v>
       </c>
       <c r="E53" t="s">
-        <v>145</v>
+        <v>456</v>
       </c>
       <c r="F53" t="s">
         <v>22</v>
@@ -7914,13 +7967,13 @@
         <v>11</v>
       </c>
       <c r="B54" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="C54" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="E54" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="F54" t="s">
         <v>22</v>
@@ -7931,13 +7984,13 @@
         <v>11</v>
       </c>
       <c r="B55" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
       <c r="C55" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
       <c r="E55" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="F55" t="s">
         <v>22</v>
@@ -7948,13 +8001,13 @@
         <v>11</v>
       </c>
       <c r="B56" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
       <c r="C56" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
       <c r="E56" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="F56" t="s">
         <v>22</v>
@@ -7965,13 +8018,13 @@
         <v>11</v>
       </c>
       <c r="B57" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
       <c r="C57" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
       <c r="E57" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="F57" t="s">
         <v>22</v>
@@ -7982,13 +8035,13 @@
         <v>11</v>
       </c>
       <c r="B58" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="C58" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="E58" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="F58" t="s">
         <v>22</v>
@@ -7999,13 +8052,13 @@
         <v>11</v>
       </c>
       <c r="B59" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="C59" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="E59" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="F59" t="s">
         <v>22</v>
@@ -8016,13 +8069,13 @@
         <v>11</v>
       </c>
       <c r="B60" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="C60" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="E60" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="F60" t="s">
         <v>22</v>
@@ -8033,13 +8086,13 @@
         <v>11</v>
       </c>
       <c r="B61" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
       <c r="C61" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
       <c r="E61" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="F61" t="s">
         <v>22</v>
@@ -8050,13 +8103,13 @@
         <v>11</v>
       </c>
       <c r="B62" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
       <c r="C62" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
       <c r="E62" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="F62" t="s">
         <v>22</v>
@@ -8067,13 +8120,13 @@
         <v>11</v>
       </c>
       <c r="B63" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
       <c r="C63" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
       <c r="E63" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="F63" t="s">
         <v>22</v>
@@ -8084,13 +8137,13 @@
         <v>11</v>
       </c>
       <c r="B64" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="C64" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="E64" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="F64" t="s">
         <v>22</v>
@@ -8101,13 +8154,13 @@
         <v>11</v>
       </c>
       <c r="B65" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="C65" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="E65" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="F65" t="s">
         <v>22</v>
@@ -8118,13 +8171,13 @@
         <v>11</v>
       </c>
       <c r="B66" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="C66" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="E66" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="F66" t="s">
         <v>22</v>
@@ -8135,13 +8188,13 @@
         <v>11</v>
       </c>
       <c r="B67" t="s">
-        <v>415</v>
+        <v>413</v>
       </c>
       <c r="C67" t="s">
-        <v>415</v>
+        <v>413</v>
       </c>
       <c r="E67" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="F67" t="s">
         <v>22</v>
@@ -8152,13 +8205,13 @@
         <v>11</v>
       </c>
       <c r="B68" t="s">
-        <v>414</v>
+        <v>415</v>
       </c>
       <c r="C68" t="s">
-        <v>414</v>
+        <v>415</v>
       </c>
       <c r="E68" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="F68" t="s">
         <v>22</v>
@@ -8169,13 +8222,13 @@
         <v>11</v>
       </c>
       <c r="B69" t="s">
-        <v>416</v>
+        <v>414</v>
       </c>
       <c r="C69" t="s">
-        <v>416</v>
+        <v>414</v>
       </c>
       <c r="E69" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="F69" t="s">
         <v>22</v>
@@ -8186,13 +8239,13 @@
         <v>11</v>
       </c>
       <c r="B70" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="C70" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="E70" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="F70" t="s">
         <v>22</v>
@@ -8203,13 +8256,13 @@
         <v>11</v>
       </c>
       <c r="B71" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
       <c r="C71" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
       <c r="E71" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="F71" t="s">
         <v>22</v>
@@ -8220,13 +8273,13 @@
         <v>11</v>
       </c>
       <c r="B72" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="C72" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="E72" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="F72" t="s">
         <v>22</v>
@@ -8237,13 +8290,13 @@
         <v>11</v>
       </c>
       <c r="B73" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
       <c r="C73" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
       <c r="E73" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="F73" t="s">
         <v>22</v>
@@ -8254,13 +8307,13 @@
         <v>11</v>
       </c>
       <c r="B74" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="C74" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="E74" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="F74" t="s">
         <v>22</v>
@@ -8271,13 +8324,13 @@
         <v>11</v>
       </c>
       <c r="B75" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="C75" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="E75" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="F75" t="s">
         <v>22</v>
@@ -8288,13 +8341,13 @@
         <v>11</v>
       </c>
       <c r="B76" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
       <c r="C76" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
       <c r="E76" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="F76" t="s">
         <v>22</v>
@@ -8305,13 +8358,13 @@
         <v>11</v>
       </c>
       <c r="B77" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
       <c r="C77" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
       <c r="E77" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="F77" t="s">
         <v>22</v>
@@ -8322,13 +8375,13 @@
         <v>11</v>
       </c>
       <c r="B78" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="C78" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="E78" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="F78" t="s">
         <v>22</v>
@@ -8339,13 +8392,13 @@
         <v>11</v>
       </c>
       <c r="B79" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="C79" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="E79" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="F79" t="s">
         <v>22</v>
@@ -8356,13 +8409,13 @@
         <v>11</v>
       </c>
       <c r="B80" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
       <c r="C80" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
       <c r="E80" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="F80" t="s">
         <v>22</v>
@@ -8373,13 +8426,13 @@
         <v>11</v>
       </c>
       <c r="B81" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
       <c r="C81" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
       <c r="E81" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="F81" t="s">
         <v>22</v>
@@ -8390,13 +8443,13 @@
         <v>11</v>
       </c>
       <c r="B82" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
       <c r="C82" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
       <c r="E82" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="F82" t="s">
         <v>22</v>
@@ -8407,13 +8460,13 @@
         <v>11</v>
       </c>
       <c r="B83" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="C83" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="E83" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="F83" t="s">
         <v>22</v>
@@ -8424,13 +8477,13 @@
         <v>11</v>
       </c>
       <c r="B84" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="C84" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="E84" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="F84" t="s">
         <v>22</v>
@@ -8441,13 +8494,13 @@
         <v>11</v>
       </c>
       <c r="B85" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
       <c r="C85" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
       <c r="E85" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="F85" t="s">
         <v>22</v>
@@ -8458,16 +8511,16 @@
         <v>11</v>
       </c>
       <c r="B86" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="C86" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="E86" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="F86" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="87" spans="1:6" x14ac:dyDescent="0.25">
@@ -8475,13 +8528,13 @@
         <v>11</v>
       </c>
       <c r="B87" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="C87" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="E87" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="F87" t="s">
         <v>23</v>
@@ -8492,13 +8545,13 @@
         <v>11</v>
       </c>
       <c r="B88" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="C88" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="E88" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="F88" t="s">
         <v>23</v>
@@ -8509,13 +8562,13 @@
         <v>11</v>
       </c>
       <c r="B89" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="C89" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="E89" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="F89" t="s">
         <v>23</v>
@@ -8526,16 +8579,16 @@
         <v>11</v>
       </c>
       <c r="B90" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="C90" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="E90" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="F90" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
     </row>
     <row r="91" spans="1:6" x14ac:dyDescent="0.25">
@@ -8543,13 +8596,13 @@
         <v>11</v>
       </c>
       <c r="B91" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
       <c r="C91" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
       <c r="E91" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="F91" t="s">
         <v>22</v>
@@ -8560,13 +8613,13 @@
         <v>11</v>
       </c>
       <c r="B92" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
       <c r="C92" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
       <c r="E92" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="F92" t="s">
         <v>22</v>
@@ -8577,13 +8630,13 @@
         <v>11</v>
       </c>
       <c r="B93" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
       <c r="C93" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
       <c r="E93" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="F93" t="s">
         <v>22</v>
@@ -8594,13 +8647,13 @@
         <v>11</v>
       </c>
       <c r="B94" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
       <c r="C94" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
       <c r="E94" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="F94" t="s">
         <v>22</v>
@@ -8611,13 +8664,13 @@
         <v>11</v>
       </c>
       <c r="B95" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="C95" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="E95" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="F95" t="s">
         <v>22</v>
@@ -8628,13 +8681,13 @@
         <v>11</v>
       </c>
       <c r="B96" t="s">
-        <v>443</v>
+        <v>442</v>
       </c>
       <c r="C96" t="s">
-        <v>443</v>
+        <v>442</v>
       </c>
       <c r="E96" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="F96" t="s">
         <v>22</v>
@@ -8645,13 +8698,13 @@
         <v>11</v>
       </c>
       <c r="B97" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
       <c r="C97" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
       <c r="E97" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="F97" t="s">
         <v>22</v>
@@ -8662,13 +8715,13 @@
         <v>11</v>
       </c>
       <c r="B98" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
       <c r="C98" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
       <c r="E98" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="F98" t="s">
         <v>22</v>
@@ -8679,13 +8732,13 @@
         <v>11</v>
       </c>
       <c r="B99" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
       <c r="C99" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
       <c r="E99" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="F99" t="s">
         <v>22</v>
@@ -8696,13 +8749,13 @@
         <v>11</v>
       </c>
       <c r="B100" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
       <c r="C100" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
       <c r="E100" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="F100" t="s">
         <v>22</v>
@@ -8713,13 +8766,13 @@
         <v>11</v>
       </c>
       <c r="B101" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
       <c r="C101" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
       <c r="E101" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="F101" t="s">
         <v>22</v>
@@ -8730,13 +8783,13 @@
         <v>11</v>
       </c>
       <c r="B102" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
       <c r="C102" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
       <c r="E102" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="F102" t="s">
         <v>22</v>
@@ -8747,13 +8800,13 @@
         <v>11</v>
       </c>
       <c r="B103" t="s">
-        <v>450</v>
+        <v>449</v>
       </c>
       <c r="C103" t="s">
-        <v>450</v>
+        <v>449</v>
       </c>
       <c r="E103" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="F103" t="s">
         <v>22</v>
@@ -8764,13 +8817,13 @@
         <v>11</v>
       </c>
       <c r="B104" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
       <c r="C104" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
       <c r="E104" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="F104" t="s">
         <v>22</v>
@@ -8781,13 +8834,13 @@
         <v>11</v>
       </c>
       <c r="B105" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
       <c r="C105" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
       <c r="E105" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="F105" t="s">
         <v>22</v>
@@ -8798,13 +8851,13 @@
         <v>11</v>
       </c>
       <c r="B106" t="s">
-        <v>453</v>
+        <v>452</v>
       </c>
       <c r="C106" t="s">
-        <v>453</v>
+        <v>452</v>
       </c>
       <c r="E106" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="F106" t="s">
         <v>22</v>
@@ -8815,15 +8868,32 @@
         <v>11</v>
       </c>
       <c r="B107" t="s">
+        <v>453</v>
+      </c>
+      <c r="C107" t="s">
+        <v>453</v>
+      </c>
+      <c r="E107" t="s">
+        <v>198</v>
+      </c>
+      <c r="F107" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="108" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A108" t="s">
+        <v>11</v>
+      </c>
+      <c r="B108" t="s">
         <v>454</v>
       </c>
-      <c r="C107" t="s">
+      <c r="C108" t="s">
         <v>454</v>
       </c>
-      <c r="E107" t="s">
+      <c r="E108" t="s">
         <v>199</v>
       </c>
-      <c r="F107" t="s">
+      <c r="F108" t="s">
         <v>22</v>
       </c>
     </row>

</xml_diff>